<commit_message>
Working on professor on new branch: Max
</commit_message>
<xml_diff>
--- a/calendarApp.xlsx
+++ b/calendarApp.xlsx
@@ -13,10 +13,10 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1618571297" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1618571297" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1618571297" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1618571297"/>
+      <pm:revision xmlns:pm="smNativeData" day="1618574911" val="982" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1618574911" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" finalRounding="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1618574911" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1618574911"/>
     </ext>
   </extLst>
 </workbook>
@@ -88,7 +88,7 @@
       <sz val="11"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1618571297" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1618574911" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="220" lang="default"/>
             <pm:cs face="Basic Roman" sz="220" lang="default"/>
             <pm:ea face="Basic Roman" sz="220" lang="default"/>
@@ -103,7 +103,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1618571297" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1618574911" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -119,7 +119,7 @@
       <sz val="14"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1618571297" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1618574911" ulstyle="none" kern="1">
             <pm:latin face="Calibri" sz="280" lang="default" weight="bold"/>
             <pm:cs face="Basic Roman" sz="280" lang="default" weight="bold"/>
             <pm:ea face="Basic Roman" sz="280" lang="default" weight="bold"/>
@@ -173,7 +173,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297"/>
+          <pm:border xmlns:pm="smNativeData" id="1618574911"/>
         </ext>
       </extLst>
     </border>
@@ -192,7 +192,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -215,7 +215,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -238,7 +238,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -261,7 +261,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
@@ -283,7 +283,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -306,7 +306,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="top" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="bottom" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
             <pm:line position="left" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
@@ -330,7 +330,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1618571297">
+          <pm:border xmlns:pm="smNativeData" id="1618574911">
             <pm:line position="right" type="1" style="0" width="30" dist="20" width2="20" rgb="000000"/>
           </pm:border>
         </ext>
@@ -340,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -350,7 +350,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -368,7 +367,7 @@
           <bgColor rgb="FFE26B0A"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1618571297" type="1" fgLvl="100" fgClr="00E26B0A" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1618574911" type="1" fgLvl="100" fgClr="00E26B0A" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -380,7 +379,7 @@
           <bgColor rgb="FFC2D69A"/>
           <extLst>
             <ext uri="smNativeData">
-              <pm:shade xmlns:pm="smNativeData" id="1618571297" type="1" fgLvl="100" fgClr="00C2D69A" bgLvl="100" bgClr="FFFFFFFF"/>
+              <pm:shade xmlns:pm="smNativeData" id="1618574911" type="1" fgLvl="100" fgClr="00C2D69A" bgLvl="100" bgClr="FFFFFFFF"/>
             </ext>
           </extLst>
         </patternFill>
@@ -390,10 +389,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1618571297" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1618574911" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1618571297" count="2">
+      <pm:colors xmlns:pm="smNativeData" id="1618574911" count="2">
         <pm:color name="Color 24" rgb="E26B0A"/>
         <pm:color name="Color 25" rgb="C2D69A"/>
       </pm:colors>
@@ -671,7 +670,7 @@
     <col min="3" max="3" width="6.553571" hidden="1" customWidth="1">
       <extLst>
         <ext uri="smNativeData">
-          <pm:columnDef xmlns:pm="smNativeData" id="1618571297" min="3" max="3" hidden="1" collapsedDB="0" collapsedOL="0"/>
+          <pm:columnDef xmlns:pm="smNativeData" id="1618574911" min="3" max="3" hidden="1" collapsedDB="0" collapsedOL="0"/>
         </ext>
       </extLst>
     </col>
@@ -721,7 +720,7 @@
         <f>WEEKDAY(B2,2)</f>
         <v>2</v>
       </c>
-      <c r="F2" s="10" t="n">
+      <c r="F2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="str">
@@ -764,7 +763,7 @@
         <f>WEEKDAY(B3,2)</f>
         <v>2</v>
       </c>
-      <c r="F3" s="10"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -781,7 +780,7 @@
       <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10" t="n">
+      <c r="F4" s="9" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="2">
@@ -817,27 +816,27 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="9"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-      <c r="O5" s="11" t="str">
+      <c r="O5" s="10" t="str">
         <f>C6</f>
         <v/>
       </c>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
     </row>
     <row r="6" spans="3:17">
       <c r="C6" t="str">
         <f>C7&amp;C8&amp;C9&amp;C10&amp;C11&amp;C12&amp;C13&amp;C14&amp;C15&amp;C16&amp;C17&amp;C18&amp;C19&amp;C20&amp;C21&amp;C22&amp;C23&amp;C24&amp;C25&amp;C26&amp;C27&amp;C28&amp;C29&amp;C30&amp;C31&amp;C32&amp;C33&amp;C34&amp;C35&amp;C36&amp;C37&amp;C38&amp;C39&amp;C40&amp;C41&amp;C42&amp;C43&amp;C44&amp;C45&amp;C46&amp;C47&amp;C48&amp;C49&amp;C50&amp;C51&amp;C52&amp;C53&amp;C54&amp;C55&amp;C56&amp;C57&amp;C58&amp;C59&amp;C60&amp;C61&amp;C62</f>
         <v/>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="9" t="n">
         <v>3</v>
       </c>
       <c r="G6" s="2">
@@ -868,9 +867,9 @@
         <f>IF(L6="","",IF(L6=$B$3,"",L6+1))</f>
         <v>44367</v>
       </c>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="8"/>
@@ -878,7 +877,7 @@
         <f>IF(G$3="v",DAY(G$2)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -892,7 +891,7 @@
         <f>IF(H$3="v",DAY(H$2)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="9" t="n">
         <v>4</v>
       </c>
       <c r="G8" s="2">
@@ -930,7 +929,7 @@
         <v/>
       </c>
       <c r="D9" s="1"/>
-      <c r="F9" s="10"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -945,7 +944,7 @@
         <v/>
       </c>
       <c r="D10" s="1"/>
-      <c r="F10" s="10" t="n">
+      <c r="F10" s="9" t="n">
         <v>5</v>
       </c>
       <c r="G10" s="2" t="str">
@@ -982,7 +981,7 @@
         <f>IF(K$3="v",DAY(K$2)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F11" s="10"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -996,7 +995,7 @@
         <f>IF(L$3="v",DAY(L$2)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="9" t="n">
         <v>6</v>
       </c>
       <c r="G12" s="2" t="str">
@@ -1034,7 +1033,7 @@
         <v/>
       </c>
       <c r="D13" s="1"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -1048,7 +1047,7 @@
         <f>IF(G$5="v",DAY(G$4)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="9" t="n">
         <v>7</v>
       </c>
       <c r="G14" s="2" t="str">
@@ -1085,7 +1084,7 @@
         <f>IF(H$5="v",DAY(H$4)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -1099,7 +1098,7 @@
         <f>IF(I$5="v",DAY(I$4)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="9" t="n">
         <v>8</v>
       </c>
       <c r="G16" s="2" t="str">
@@ -1136,7 +1135,7 @@
         <f>IF(J$5="v",DAY(J$4)&amp;";","")</f>
         <v/>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -1450,7 +1449,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1618571297" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1618574911" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1459,14 +1458,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1618571297" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1618571297" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1618574911" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1618574911" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1618571297" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1618574911" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>